<commit_message>
fixed encoding issues with reading grim_books, added functions to spreadsheet
</commit_message>
<xml_diff>
--- a/scriptsInputOutput.xlsx
+++ b/scriptsInputOutput.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="functions" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -227,6 +228,285 @@
   </si>
   <si>
     <t xml:space="preserve">Data/Processed/pa_melbourne.Rds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runScenario.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/trips_prep.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateVistaTrips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_VISTA_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Travelsurvey/VISTA12-18/H_VISTA_1218_V1.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person_VISTA_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Travelsurvey/VISTA12-18/P_VISTA1218_V1.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trip_VISTA_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Travelsurvey/VISTA12-18/T_VISTA1218_V1.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/scenarios.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateScenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trips_melbourne_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/synthetic_pop.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateTravelData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/travel_data.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ses_index_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Travelsurvey/ABS SEIFA/ses.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculatePersonsTravelScenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel_data_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persons_travel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/persons_travel.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scenario_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculatePersonsPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pa_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/persons_pa.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculatePersonsMatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persons_matched</t>
+  </si>
+  <si>
+    <t xml:space="preserve">persons_travel_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runDataPrepMSLT.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/death_rates_prep.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateDeathRates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population_deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death_rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/ithim_gbd_prep.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateGBDandPopulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbd_melbourne_ithimr_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBDandPopulation[[1]] (gbd_melbourne)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population_melbourne_abs_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBDandPopulation[[2]] (population_melbourne)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateDiseaseNames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbd_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disease_names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disease_outcomes_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateGBDwider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbd_wider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/gbd_wider.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateMSLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population_melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mslt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/mslt/mslt_df.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deaths_melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dismod_output_cancers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/dismod_output_cancers.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dismod_output_non_cancers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/dismod_output_non_cancers.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/trends_prep.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateDiseaseTrends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incidence_trends_cancers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/aihw/cancer_incidence_AIHW_with_projections.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trends_diseases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mortality_trends_cancers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/aihw/trends/cancers_trends_mortality_aihw.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incidence_trends_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/mslt/incidence_trends_f.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trends_cvd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/aihw/trends/cardiovascular_disease_trends_aihw.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incidence_trends_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/mslt/incidence_trends_m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grim_books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/aihw/trends/grim_books.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mortality_trends_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/mslt/mortality_trends_f.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trends_diabetes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/aihw/trends/diabetes_trends_aihw.xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mortality_trends_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data/Processed/mslt/mortality_trends_m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT YET REFERENCED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/data_prep/injuries_prep.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculateInjuries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accident_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">injuries_melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accident_event_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicle_location</t>
   </si>
 </sst>
 </file>
@@ -236,7 +516,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -265,8 +545,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,25 +568,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF77BC65"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEC9BA4"/>
-        <bgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFFFA6A6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD4EA6B"/>
         <bgColor rgb="FFE8F2A1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE8F2A1"/>
-        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
     <fill>
@@ -306,7 +592,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -324,13 +610,49 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDEE6EF"/>
-        <bgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
         <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDEE6EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFFFFFA6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFB4C7DC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFAA95"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFE8F2A1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFFA6A6"/>
       </patternFill>
     </fill>
   </fills>
@@ -396,7 +718,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -457,23 +779,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,15 +799,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,11 +815,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,12 +835,96 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -537,7 +939,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -554,15 +956,15 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FFE8F2A1"/>
       <rgbColor rgb="FFDEE6EF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFEC9BA4"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFD4EA6B"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -571,10 +973,10 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFDDE8CB"/>
-      <rgbColor rgb="FFE8F2A1"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFEC9BA4"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFFFA6"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -604,13 +1006,13 @@
   </sheetPr>
   <dimension ref="A3:E59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="52.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="36.14"/>
@@ -675,40 +1077,40 @@
       <c r="D8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -732,7 +1134,7 @@
       <c r="D14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="21" t="s">
         <v>23</v>
       </c>
     </row>
@@ -750,19 +1152,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
@@ -770,7 +1172,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="13"/>
-      <c r="D19" s="25"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -779,20 +1181,20 @@
       <c r="B21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="18"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
@@ -800,16 +1202,16 @@
         <v>35</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="25"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="11"/>
@@ -817,7 +1219,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="25"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
@@ -833,35 +1235,35 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
@@ -869,7 +1271,7 @@
         <v>42</v>
       </c>
       <c r="C33" s="13"/>
-      <c r="D33" s="25"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -884,18 +1286,18 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C37" s="13"/>
-      <c r="D37" s="25"/>
+      <c r="D37" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -940,18 +1342,18 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="13"/>
-      <c r="D46" s="25"/>
+      <c r="D46" s="23"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
@@ -971,46 +1373,46 @@
       <c r="D52" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="18" t="s">
+      <c r="C53" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D53" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="18" t="s">
+      <c r="C54" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="18"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
     </row>
     <row r="56" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="29" t="s">
         <v>63</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="25"/>
+      <c r="D56" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -1025,7 +1427,7 @@
       <c r="D58" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E58" s="23" t="s">
+      <c r="E58" s="21" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1034,7 +1436,7 @@
       <c r="C59" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="25"/>
+      <c r="D59" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1045,4 +1447,603 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:G52"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="744" topLeftCell="A10" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.33"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="22"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="22"/>
+      <c r="C17" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="22"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="22"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="22"/>
+      <c r="C32" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" s="33"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="45" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
started work on mslt_code
</commit_message>
<xml_diff>
--- a/scriptsInputOutput.xlsx
+++ b/scriptsInputOutput.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="165">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -365,13 +365,16 @@
     <t xml:space="preserve">gbd_melbourne_ithimr_location</t>
   </si>
   <si>
-    <t xml:space="preserve">GBDandPopulation[[1]] (gbd_melbourne)</t>
+    <t xml:space="preserve">GBDandPopulation</t>
   </si>
   <si>
     <t xml:space="preserve">population_melbourne_abs_location</t>
   </si>
   <si>
-    <t xml:space="preserve">GBDandPopulation[[2]] (population_melbourne)</t>
+    <t xml:space="preserve">gbd_melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">population_melbourne</t>
   </si>
   <si>
     <t xml:space="preserve">calculateDiseaseNames</t>
@@ -398,9 +401,6 @@
     <t xml:space="preserve">calculateMSLT</t>
   </si>
   <si>
-    <t xml:space="preserve">population_melbourne</t>
-  </si>
-  <si>
     <t xml:space="preserve">mslt</t>
   </si>
   <si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t xml:space="preserve">Data/Processed/mslt/mortality_trends_m.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts/mslt_code.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disease_outcomes_lookup_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matched_pop_location</t>
   </si>
   <si>
     <t xml:space="preserve">NOT YET REFERENCED</t>
@@ -516,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -546,6 +555,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -558,7 +573,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,7 +595,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD4EA6B"/>
-        <bgColor rgb="FFE8F2A1"/>
+        <bgColor rgb="FFBBE33D"/>
       </patternFill>
     </fill>
     <fill>
@@ -655,6 +670,12 @@
         <bgColor rgb="FFFFA6A6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor rgb="FFD4EA6B"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
@@ -718,7 +739,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -895,6 +916,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -907,11 +932,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,7 +964,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -980,14 +1033,14 @@
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF77BC65"/>
+      <rgbColor rgb="FFBBE33D"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFBF819E"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -1454,22 +1507,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G52"/>
+  <dimension ref="B1:G56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="744" topLeftCell="A10" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="732" topLeftCell="A4" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1701,7 +1754,7 @@
       <c r="F19" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1711,14 +1764,14 @@
       <c r="D20" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="45" t="s">
         <v>97</v>
       </c>
       <c r="F20" s="35"/>
       <c r="G20" s="35"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="46" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1738,7 +1791,7 @@
       <c r="F24" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="47" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1755,117 +1808,115 @@
       <c r="E26" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="49"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="47" t="s">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="52" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="33" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="48" t="s">
+      <c r="C30" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="D30" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="33" t="s">
+      <c r="F30" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="22"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22"/>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="35"/>
+      <c r="D31" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" s="41" t="s">
-        <v>123</v>
-      </c>
+      <c r="E31" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="22"/>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="53" t="s">
         <v>124</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="G32" s="33" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="C33" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>123</v>
+        <v>128</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>6</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -1874,168 +1925,206 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>124</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E37" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="33" t="s">
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C39" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D39" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E39" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="F38" s="51" t="s">
+      <c r="F39" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="G38" s="33"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" s="22" t="s">
-        <v>141</v>
-      </c>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E42" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F42" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="G42" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35" t="s">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E43" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F43" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G43" s="35" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="45" t="s">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="33" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="33" t="s">
+      <c r="C45" s="33"/>
+      <c r="D45" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="E45" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="E46" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="E49" s="33" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="F49" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="G49" s="33" t="s">
+      <c r="F53" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" s="33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="E50" s="22" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="E51" s="22" t="s">
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="E52" s="35" t="s">
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="E56" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>